<commit_message>
sinkron dgn lp ucup
</commit_message>
<xml_diff>
--- a/yabuki/database/orang/aulia/exel_boomber_aulia/F2 Aulia Database Notel [Kenal Nama].xlsx
+++ b/yabuki/database/orang/aulia/exel_boomber_aulia/F2 Aulia Database Notel [Kenal Nama].xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ucup_d\yabuki\database\orang\aulia\exel_boomber_aulia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B822D09C-2BE0-4D7E-BA12-DBA91573534B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50DEACAE-4AB8-4A6B-8CAC-222CAABE2502}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="1515" windowWidth="12660" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3585" yWindow="3585" windowWidth="12660" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1232" uniqueCount="1053">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1258" uniqueCount="1079">
   <si>
     <t>Keterangan</t>
   </si>
@@ -3192,6 +3192,84 @@
   </si>
   <si>
     <t>Kak Alif</t>
+  </si>
+  <si>
+    <t>Ibu lely</t>
+  </si>
+  <si>
+    <t>+62 853-2730-9905</t>
+  </si>
+  <si>
+    <t>Bapak subadri</t>
+  </si>
+  <si>
+    <t>+62 811-2013-444</t>
+  </si>
+  <si>
+    <t>Ibu dwi</t>
+  </si>
+  <si>
+    <t>+62 853-2732-8254</t>
+  </si>
+  <si>
+    <t>Ibu fitria</t>
+  </si>
+  <si>
+    <t>+62 853-2248-4660</t>
+  </si>
+  <si>
+    <t>Mas rohmat</t>
+  </si>
+  <si>
+    <t>+62 831-2330-0404</t>
+  </si>
+  <si>
+    <t>Bapak didin</t>
+  </si>
+  <si>
+    <t>+62 856-4981-2088</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bapak fajar </t>
+  </si>
+  <si>
+    <t>+62 811-2013-699</t>
+  </si>
+  <si>
+    <t>Mba aurel</t>
+  </si>
+  <si>
+    <t>+62 813-6538-5112</t>
+  </si>
+  <si>
+    <t>Mas rian</t>
+  </si>
+  <si>
+    <t>+62 812-4523-7524</t>
+  </si>
+  <si>
+    <t>Mas farhan</t>
+  </si>
+  <si>
+    <t>+62 853-2249-8696</t>
+  </si>
+  <si>
+    <t>Ibu pipih</t>
+  </si>
+  <si>
+    <t>+62 853-2249-9507</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bapak aprio </t>
+  </si>
+  <si>
+    <t>+62 856-4986-5523</t>
+  </si>
+  <si>
+    <t>Mas taslim</t>
+  </si>
+  <si>
+    <t>+62 812-4464-5894</t>
   </si>
 </sst>
 </file>
@@ -3265,7 +3343,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3318,6 +3396,11 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3609,8 +3692,8 @@
   </sheetPr>
   <dimension ref="A1:G904"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A586" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:D607"/>
+    <sheetView tabSelected="1" topLeftCell="A604" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D616" sqref="D616"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -13681,112 +13764,216 @@
       <c r="F607" s="7"/>
     </row>
     <row r="608" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A608" s="3"/>
-      <c r="B608" s="4"/>
-      <c r="C608" s="5"/>
-      <c r="D608" s="6"/>
+      <c r="A608" s="3">
+        <v>676</v>
+      </c>
+      <c r="B608" s="21">
+        <v>44596</v>
+      </c>
+      <c r="C608" s="20" t="s">
+        <v>1068</v>
+      </c>
+      <c r="D608" s="14" t="s">
+        <v>1067</v>
+      </c>
       <c r="E608" s="7"/>
       <c r="F608" s="7"/>
       <c r="G608" s="7"/>
     </row>
     <row r="609" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A609" s="3"/>
-      <c r="B609" s="4"/>
-      <c r="C609" s="5"/>
-      <c r="D609" s="11"/>
+      <c r="A609" s="3">
+        <v>677</v>
+      </c>
+      <c r="B609" s="21">
+        <v>44594</v>
+      </c>
+      <c r="C609" s="20" t="s">
+        <v>1066</v>
+      </c>
+      <c r="D609" s="14" t="s">
+        <v>1065</v>
+      </c>
       <c r="E609" s="7"/>
       <c r="F609" s="7"/>
     </row>
     <row r="610" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A610" s="3"/>
-      <c r="B610" s="4"/>
-      <c r="C610" s="5"/>
-      <c r="D610" s="6"/>
+      <c r="A610" s="3">
+        <v>678</v>
+      </c>
+      <c r="B610" s="21">
+        <v>44600</v>
+      </c>
+      <c r="C610" s="20" t="s">
+        <v>1064</v>
+      </c>
+      <c r="D610" s="14" t="s">
+        <v>1063</v>
+      </c>
       <c r="E610" s="7"/>
       <c r="F610" s="7"/>
       <c r="G610" s="7"/>
     </row>
     <row r="611" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A611" s="3"/>
-      <c r="B611" s="4"/>
-      <c r="C611" s="5"/>
-      <c r="D611" s="11"/>
+      <c r="A611" s="3">
+        <v>679</v>
+      </c>
+      <c r="B611" s="21">
+        <v>44609</v>
+      </c>
+      <c r="C611" s="20" t="s">
+        <v>1062</v>
+      </c>
+      <c r="D611" s="14" t="s">
+        <v>1061</v>
+      </c>
       <c r="E611" s="7"/>
       <c r="F611" s="7"/>
     </row>
     <row r="612" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A612" s="3"/>
-      <c r="B612" s="4"/>
-      <c r="C612" s="5"/>
-      <c r="D612" s="6"/>
+      <c r="A612" s="3">
+        <v>680</v>
+      </c>
+      <c r="B612" s="21">
+        <v>44613</v>
+      </c>
+      <c r="C612" s="20" t="s">
+        <v>1060</v>
+      </c>
+      <c r="D612" s="14" t="s">
+        <v>1059</v>
+      </c>
       <c r="E612" s="7"/>
       <c r="F612" s="7"/>
       <c r="G612" s="7"/>
     </row>
     <row r="613" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A613" s="3"/>
-      <c r="B613" s="4"/>
-      <c r="C613" s="5"/>
-      <c r="D613" s="11"/>
+      <c r="A613" s="3">
+        <v>681</v>
+      </c>
+      <c r="B613" s="21">
+        <v>44630</v>
+      </c>
+      <c r="C613" s="20" t="s">
+        <v>1058</v>
+      </c>
+      <c r="D613" s="14" t="s">
+        <v>1057</v>
+      </c>
       <c r="E613" s="7"/>
       <c r="F613" s="7"/>
     </row>
     <row r="614" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A614" s="3"/>
-      <c r="B614" s="4"/>
-      <c r="C614" s="5"/>
-      <c r="D614" s="6"/>
+      <c r="A614" s="3">
+        <v>682</v>
+      </c>
+      <c r="B614" s="21">
+        <v>44594</v>
+      </c>
+      <c r="C614" s="20" t="s">
+        <v>1056</v>
+      </c>
+      <c r="D614" s="14" t="s">
+        <v>1055</v>
+      </c>
       <c r="E614" s="7"/>
       <c r="F614" s="7"/>
       <c r="G614" s="7"/>
     </row>
     <row r="615" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A615" s="3"/>
-      <c r="B615" s="4"/>
-      <c r="C615" s="5"/>
-      <c r="D615" s="11"/>
+      <c r="A615" s="3">
+        <v>683</v>
+      </c>
+      <c r="B615" s="21">
+        <v>44624</v>
+      </c>
+      <c r="C615" s="20" t="s">
+        <v>1054</v>
+      </c>
+      <c r="D615" s="14" t="s">
+        <v>1053</v>
+      </c>
       <c r="E615" s="7"/>
       <c r="F615" s="7"/>
     </row>
     <row r="616" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A616" s="3"/>
-      <c r="B616" s="4"/>
-      <c r="C616" s="5"/>
-      <c r="D616" s="6"/>
+      <c r="A616" s="3">
+        <v>684</v>
+      </c>
+      <c r="B616" s="21">
+        <v>44579</v>
+      </c>
+      <c r="C616" s="14" t="s">
+        <v>1078</v>
+      </c>
+      <c r="D616" s="14" t="s">
+        <v>1077</v>
+      </c>
       <c r="E616" s="7"/>
       <c r="F616" s="7"/>
       <c r="G616" s="7"/>
     </row>
     <row r="617" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A617" s="3"/>
-      <c r="B617" s="4"/>
-      <c r="C617" s="5"/>
-      <c r="D617" s="11"/>
+      <c r="A617" s="3">
+        <v>685</v>
+      </c>
+      <c r="B617" s="21">
+        <v>44580</v>
+      </c>
+      <c r="C617" s="14" t="s">
+        <v>1076</v>
+      </c>
+      <c r="D617" s="14" t="s">
+        <v>1075</v>
+      </c>
       <c r="E617" s="7"/>
       <c r="F617" s="7"/>
     </row>
     <row r="618" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A618" s="3"/>
-      <c r="B618" s="4"/>
-      <c r="C618" s="5"/>
-      <c r="D618" s="6"/>
+      <c r="A618" s="3">
+        <v>686</v>
+      </c>
+      <c r="B618" s="21">
+        <v>44622</v>
+      </c>
+      <c r="C618" s="14" t="s">
+        <v>1074</v>
+      </c>
+      <c r="D618" s="14" t="s">
+        <v>1073</v>
+      </c>
       <c r="E618" s="7"/>
       <c r="F618" s="7"/>
       <c r="G618" s="7"/>
     </row>
     <row r="619" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A619" s="3"/>
-      <c r="B619" s="4"/>
-      <c r="C619" s="5"/>
-      <c r="D619" s="11"/>
+      <c r="A619" s="3">
+        <v>687</v>
+      </c>
+      <c r="B619" s="21">
+        <v>44627</v>
+      </c>
+      <c r="C619" s="14" t="s">
+        <v>1072</v>
+      </c>
+      <c r="D619" s="14" t="s">
+        <v>1071</v>
+      </c>
       <c r="E619" s="7"/>
       <c r="F619" s="7"/>
     </row>
     <row r="620" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A620" s="3"/>
-      <c r="B620" s="4"/>
-      <c r="C620" s="5"/>
-      <c r="D620" s="6"/>
+      <c r="A620" s="3">
+        <v>688</v>
+      </c>
+      <c r="B620" s="21">
+        <v>44597</v>
+      </c>
+      <c r="C620" s="22" t="s">
+        <v>1070</v>
+      </c>
+      <c r="D620" s="14" t="s">
+        <v>1069</v>
+      </c>
       <c r="E620" s="7"/>
       <c r="F620" s="7"/>
       <c r="G620" s="7"/>

</xml_diff>